<commit_message>
EPBDS: added validation phase for mapping subproject. Added base implementation of bean validator for mapping definitions validation (a field hierarchy check, a custom converters check and field mapping condition check).
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/OneToOneMappingsTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev.test/src/test/resources/org/openl/rules/mapping/OneToOneMappingsTest.xlsx
@@ -46,9 +46,6 @@
     <t>oneWay</t>
   </si>
   <si>
-    <t>Data Mapping mappings1</t>
-  </si>
-  <si>
     <t>Method String myConvertMethod(String[] source, String destination )</t>
   </si>
   <si>
@@ -93,46 +90,49 @@
     <t>import</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>org.openl.rules.mapping</t>
+  </si>
+  <si>
+    <t>org.openl.rules.mapping.to</t>
+  </si>
+  <si>
+    <t>convertMethodAB</t>
+  </si>
+  <si>
+    <t>convertMethodBA</t>
+  </si>
+  <si>
+    <t>anInt</t>
+  </si>
+  <si>
+    <t>aString</t>
+  </si>
+  <si>
+    <t>b.aString</t>
+  </si>
+  <si>
+    <t>anInteger</t>
+  </si>
+  <si>
+    <t>b.anInteger</t>
+  </si>
+  <si>
+    <t>aStringArray</t>
+  </si>
+  <si>
+    <t>aList</t>
+  </si>
+  <si>
+    <t>aStringArray[1]</t>
+  </si>
+  <si>
+    <t>Data Mapping mappings1</t>
+  </si>
+  <si>
     <t>Data Mapping mappings2</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>org.openl.rules.mapping</t>
-  </si>
-  <si>
-    <t>org.openl.rules.mapping.to</t>
-  </si>
-  <si>
-    <t>convertMethodAB</t>
-  </si>
-  <si>
-    <t>convertMethodBA</t>
-  </si>
-  <si>
-    <t>anInt</t>
-  </si>
-  <si>
-    <t>aString</t>
-  </si>
-  <si>
-    <t>b.aString</t>
-  </si>
-  <si>
-    <t>anInteger</t>
-  </si>
-  <si>
-    <t>b.anInteger</t>
-  </si>
-  <si>
-    <t>aStringArray</t>
-  </si>
-  <si>
-    <t>aList</t>
-  </si>
-  <si>
-    <t>aStringArray[1]</t>
   </si>
 </sst>
 </file>
@@ -536,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C4:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,31 +557,31 @@
   <sheetData>
     <row r="4" spans="3:9">
       <c r="C4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="3:9" ht="149.25" customHeight="1">
       <c r="C5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="8"/>
     </row>
     <row r="7" spans="3:9">
       <c r="C7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="3:9" ht="78.75" customHeight="1">
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="8"/>
     </row>
     <row r="12" spans="3:9">
       <c r="C12" s="5" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -604,10 +604,10 @@
         <v>3</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>9</v>
@@ -644,10 +644,10 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="3:9">
@@ -658,10 +658,10 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="3:9">
@@ -672,10 +672,10 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -689,10 +689,10 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G18" t="s">
         <v>6</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="22" spans="3:9">
       <c r="C22" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -726,10 +726,10 @@
         <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>9</v>
@@ -760,13 +760,13 @@
     </row>
     <row r="25" spans="3:9">
       <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" t="s">
         <v>5</v>
@@ -777,47 +777,47 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="3:9">
       <c r="C27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="3:9">
       <c r="C30" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="3:9">
       <c r="C31" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="3:9">
       <c r="C32" s="7"/>
       <c r="D32" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>